<commit_message>
added zero to all none and nan
</commit_message>
<xml_diff>
--- a/data/trial.xlsx
+++ b/data/trial.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,454 +434,570 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="n">
-        <v>3</v>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>budget_line</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>budget</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>income</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>expenses</t>
+        </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>BUDGET_LINE</t>
-        </is>
+      <c r="A2" t="n">
+        <v>10</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BUDGET</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Income</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Expense</t>
-        </is>
+          <t>AmbassadorChristmas</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>AmbassadorChristmas</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
+          <t>AmbassadorOctoberfest</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>AmbassadorOctoberfest</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
+          <t>AmbassadorSummer</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>AmbassadorSummer</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
+          <t>BackPackProgram</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>BackPackProgram</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
+          <t>BoyScouts</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>BoyScouts</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
+          <t>Breakfast 25</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1698.23</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Breakfast 25</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr"/>
+          <t>Building Rental</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
       <c r="D8" t="n">
-        <v>1698.23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Building Rental</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
+          <t>CampStix</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>CampStix</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
+          <t>CancerHouse</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>CancerHouse</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
+          <t>CAREMD19</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>CAREMD19</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
+          <t>CascadeMedicalFoundation</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>CascadeMedicalFoundation</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
+          <t>ChamberCommerceDues</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ChamberCommerceDues</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
+          <t>ChestnutScoring</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ChestnutScoring</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
+          <t>Clothing4Kids</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Clothing4Kids</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
+          <t>CreechScholarship</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>CreechScholarship</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
+          <t>CubScouts</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>CubScouts</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
+          <t>Donations</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Donations</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
+          <t>EasterEggHunt</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>EasterEggHunt</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
+          <t>EyeGlasses &amp; HearingAids</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>EyeGlasses &amp; HearingAids</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
+          <t>Health Permit</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Health Permit</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
+          <t>InsuranceOnBuildingContents</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>220</v>
+        <v>230</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>InsuranceOnBuildingContents</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr"/>
+          <t>InterestOnBankAccounts</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>230</v>
+        <v>240</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>InterestOnBankAccounts</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr"/>
+          <t>LCIF</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>240</v>
+        <v>250</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>LCIF</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr"/>
+          <t>LeavenworthActivityFee</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>250</v>
+        <v>260</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>LeavenworthActivityFee</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr"/>
+          <t>MEND</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>260</v>
+        <v>270</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>MEND</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr"/>
+          <t>MiscCommunitySupport</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>MiscCommunitySupport</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr"/>
+          <t>MountainMeadows</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>280</v>
+        <v>290</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>MountainMeadows</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr"/>
-      <c r="D29" t="inlineStr"/>
+          <t>PublicRelations</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>290</v>
+        <v>300</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>PublicRelations</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr"/>
-      <c r="D30" t="inlineStr"/>
+          <t>Scholarships</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>300</v>
+        <v>320</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Scholarships</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr"/>
-      <c r="D31" t="inlineStr"/>
+          <t>SwimTeamFundraiser (hot dogs)</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" t="n">
+        <v>400</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>320</v>
+        <v>330</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>SwimTeamFundraiser (hot dogs)</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr"/>
+          <t>VisionScreening</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>0</v>
+      </c>
       <c r="D32" t="n">
-        <v>400</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>VisionScreening</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr"/>
-      <c r="D33" t="inlineStr"/>
+          <t>YouthExchange</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" t="n">
+        <v>252</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>340</v>
+        <v>350</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>YouthExchange</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr"/>
+          <t>YouthSports</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>0</v>
+      </c>
       <c r="D34" t="n">
-        <v>252</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>350</v>
+        <v>360</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>YouthSports</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr"/>
-      <c r="D35" t="inlineStr"/>
-    </row>
-    <row r="36">
-      <c r="A36" t="n">
-        <v>360</v>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
           <t>White Cane</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr"/>
-      <c r="D36" t="inlineStr"/>
+      <c r="C35" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>